<commit_message>
excel aggiornato con dati coerenti
</commit_message>
<xml_diff>
--- a/pythonProject/input/Input modello.xlsx
+++ b/pythonProject/input/Input modello.xlsx
@@ -1036,7 +1036,7 @@
   <dimension ref="A1:AE1000"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1251,9 +1251,7 @@
       <c r="K4" s="12">
         <v>1</v>
       </c>
-      <c r="L4" s="16">
-        <v>44197</v>
-      </c>
+      <c r="L4" s="16"/>
       <c r="M4" s="13"/>
       <c r="N4" s="13"/>
       <c r="O4" s="15"/>

</xml_diff>